<commit_message>
Mise à jour de partitions
</commit_message>
<xml_diff>
--- a/Table des accords.xlsx
+++ b/Table des accords.xlsx
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AL16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AN5" sqref="AN5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScale="160" zoomScaleNormal="130" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,7 +940,7 @@
         <v>4</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="12" t="s">
@@ -1641,7 +1641,7 @@
         <v>4</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="8" t="s">

</xml_diff>